<commit_message>
Comparison of Openchain Translation
</commit_message>
<xml_diff>
--- a/misc/OpenChain翻訳アプローチ比較20171101.xlsx
+++ b/misc/OpenChain翻訳アプローチ比較20171101.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WINXP\201710\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WINXP\201705\lf-j\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12150"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="English" sheetId="2" r:id="rId1"/>
+    <sheet name="Japanese" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="86">
   <si>
     <t>日本語</t>
     <rPh sb="0" eb="3">
@@ -52,9 +53,6 @@
       <t>ゴ</t>
     </rPh>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>簡体/繁体中国語</t>
   </si>
   <si>
     <t>OpenChain 言語翻訳の比較</t>
@@ -126,10 +124,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>4+</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>なし</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -193,11 +187,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>人数
-（Contributor)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2017/11/1現在</t>
     <rPh sb="9" eb="11">
       <t>ゲンザイ</t>
@@ -289,6 +278,245 @@
   </si>
   <si>
     <t>- Onboading matrialのみ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[*1] 以下サイトにの翻訳者（メンテな含む）https://www.openchainproject.org/translations </t>
+    <rPh sb="5" eb="7">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>ホンヤクシャ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>フク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>翻訳者人数</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>*1</t>
+    </r>
+    <rPh sb="0" eb="3">
+      <t>ホンヤクシャ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Github Repoのコントリビュータ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>繁体中国語</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>簡体中国語</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Number of Translator</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>*1</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Contributor(s) in Github Repo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Used Tools </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Copyright Declaration</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Info </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>As of 1st November 2017</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Comparison of OpenChain Translation approach</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Japanease</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Korean</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Italian</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Simplified Chinese</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Traditional Chinese</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>French</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Polish</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Spanish</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Geremany</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Portuguese</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3
+(Incld.Shane)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>N/A
+(Empty)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1
+(Mark Gisi)※</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1
+(Mark Gisi )</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4
+(Mark)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1名
+(Shane)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1
+(Mark)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OmegaT
++Manual work</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OmegaT
++ Manual Work</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edit .md -&gt;tml</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Nothinng</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Nothing
+(See below)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Nothing</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Manual work(Maybe)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Manual work  (ODT)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[*1] Translators are referred in the following URL(Including Maintener)https://www.openchainproject.org/translations </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">- About Curriculum, tool seems to be switched to OmegaT forv.1.1 
+- in old version of Curriculm, copyright was declared. </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>- Auther names are written in Readme.(not as copyright notice)
+-License Information is very friendly.
+https://github.com/OpenChain-Project/Specification-Translation-IT/blob/master/LICENSE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-License Information is very friendly same as Italian team. (Mark have made this info)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">-Actural work seems to be done separately from Github.and Shane upload release version as a proxy.
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">-Actural work seems to be done separately from Github.and Mark upload release version as a proxy. 
+-PDF/Word/ODT files are broken? (can't be open)
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">-Actural work seems to be done separately from Github.and Mark upload release version as a proxy.
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>- Only Onboading matrial</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -296,7 +524,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +570,14 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -351,7 +587,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -501,13 +737,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -526,82 +775,100 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -887,366 +1154,926 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:S10"/>
+  <dimension ref="A2:U13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.25" style="1" customWidth="1"/>
-    <col min="2" max="19" width="11.25" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9" style="1"/>
+    <col min="2" max="21" width="11.25" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
-        <v>26</v>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="12"/>
-      <c r="B5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6" t="s">
+    <row r="4" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="23"/>
+      <c r="B5" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="28"/>
+      <c r="N5" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" s="28"/>
+      <c r="P5" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" s="28"/>
+      <c r="T5" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" s="28"/>
+    </row>
+    <row r="6" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="24"/>
+      <c r="B6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="34">
+        <v>5</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36">
+        <v>2</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="36">
+        <v>2</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="36">
+        <v>3</v>
+      </c>
+      <c r="I7" s="37"/>
+      <c r="J7" s="36">
+        <v>6</v>
+      </c>
+      <c r="K7" s="37"/>
+      <c r="L7" s="36">
+        <v>3</v>
+      </c>
+      <c r="M7" s="37"/>
+      <c r="N7" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" s="37"/>
+      <c r="P7" s="36">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="36">
+        <v>2</v>
+      </c>
+      <c r="S7" s="37"/>
+      <c r="T7" s="36">
+        <v>3</v>
+      </c>
+      <c r="U7" s="37"/>
+    </row>
+    <row r="8" spans="1:21" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="15">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>5</v>
+      </c>
+      <c r="D8" s="33">
         <v>1</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" s="7"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="18" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="13"/>
-      <c r="B6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>13</v>
+    <row r="9" spans="1:21" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="18" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P7" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R7" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="S7" s="31" t="s">
-        <v>22</v>
+    <row r="10" spans="1:21" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="S10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="18" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R8" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="S8" s="31" t="s">
-        <v>22</v>
-      </c>
+    <row r="11" spans="1:21" s="5" customFormat="1" ht="183" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="20"/>
+      <c r="L11" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="M11" s="20"/>
+      <c r="N11" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="S11" s="20"/>
+      <c r="T11" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="U11" s="20"/>
     </row>
-    <row r="9" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R9" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="S9" s="31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" s="5" customFormat="1" ht="183" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="25"/>
-      <c r="L10" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="25"/>
-      <c r="P10" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="S10" s="25"/>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="R10:S10"/>
+  <mergeCells count="36">
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="L5:M5"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:S5"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="61" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;F</oddHeader>
+    <oddFooter>&amp;P / &amp;N ページ</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:U13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7:O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.25" style="1" customWidth="1"/>
+    <col min="2" max="21" width="11.25" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="23"/>
+      <c r="B5" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="28"/>
+      <c r="N5" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="28"/>
+      <c r="P5" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S5" s="28"/>
+      <c r="T5" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="U5" s="28"/>
+    </row>
+    <row r="6" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="24"/>
+      <c r="B6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="34">
+        <v>5</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36">
+        <v>2</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="36">
+        <v>2</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="36">
+        <v>3</v>
+      </c>
+      <c r="I7" s="37"/>
+      <c r="J7" s="36">
+        <v>6</v>
+      </c>
+      <c r="K7" s="37"/>
+      <c r="L7" s="36">
+        <v>3</v>
+      </c>
+      <c r="M7" s="37"/>
+      <c r="N7" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" s="37"/>
+      <c r="P7" s="36">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="36">
+        <v>2</v>
+      </c>
+      <c r="S7" s="37"/>
+      <c r="T7" s="36">
+        <v>3</v>
+      </c>
+      <c r="U7" s="37"/>
+    </row>
+    <row r="8" spans="1:21" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="13">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>5</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="5" customFormat="1" ht="183" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="20"/>
+      <c r="L11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="20"/>
+      <c r="N11" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="20"/>
+      <c r="T11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="U11" s="20"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="D11:E11"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;F</oddHeader>
     <oddFooter>&amp;P / &amp;N ページ</oddFooter>

</xml_diff>